<commit_message>
nina pairwise new launch
</commit_message>
<xml_diff>
--- a/05-Amazon_MTurk_expert_response_30cow_pairwise/results/Amazon_HIT_expert_submission_track_master.xlsx
+++ b/05-Amazon_MTurk_expert_response_30cow_pairwise/results/Amazon_HIT_expert_submission_track_master.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ubcca-my.sharepoint.com/personal/skysheng_student_ubc_ca/Documents/R package project and Git/lameness_rank/05-Amazon_MTurk_expert_response_30cow_pairwise/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="47" documentId="13_ncr:1_{F1D378CC-E7F6-D04B-9DEF-7DD515FBB73B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A9069456-4A5E-734C-B7E3-97A3C66D976F}"/>
+  <xr:revisionPtr revIDLastSave="51" documentId="13_ncr:1_{F1D378CC-E7F6-D04B-9DEF-7DD515FBB73B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{77C7A4CB-A3EC-9A47-BD09-BEC2CCA89136}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17180" xr2:uid="{40C02EE5-B5BA-A247-AF77-BCFF49CE157A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="44">
   <si>
     <t>Date</t>
   </si>
@@ -156,6 +156,18 @@
   </si>
   <si>
     <t>RD</t>
+  </si>
+  <si>
+    <t>paiewise</t>
+  </si>
+  <si>
+    <t>Sep-22-2023</t>
+  </si>
+  <si>
+    <t>NV</t>
+  </si>
+  <si>
+    <t>all_submitted_tracker_ninaSep-22-2023</t>
   </si>
 </sst>
 </file>
@@ -516,10 +528,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AFACC2C-8593-5541-A725-7B0C1E651424}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -720,6 +732,20 @@
         <v>36</v>
       </c>
     </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" t="s">
+        <v>43</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
nina response all collected
</commit_message>
<xml_diff>
--- a/05-Amazon_MTurk_expert_response_30cow_pairwise/results/Amazon_HIT_expert_submission_track_master.xlsx
+++ b/05-Amazon_MTurk_expert_response_30cow_pairwise/results/Amazon_HIT_expert_submission_track_master.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ubcca-my.sharepoint.com/personal/skysheng_student_ubc_ca/Documents/R package project and Git/lameness_rank/05-Amazon_MTurk_expert_response_30cow_pairwise/results/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/skysheng/Library/CloudStorage/OneDrive-UBC/R package project and Git/lameness_rank/05-Amazon_MTurk_expert_response_30cow_pairwise/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="51" documentId="13_ncr:1_{F1D378CC-E7F6-D04B-9DEF-7DD515FBB73B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{77C7A4CB-A3EC-9A47-BD09-BEC2CCA89136}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A04707D-2468-8E4C-B91A-D81291A791A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17180" xr2:uid="{40C02EE5-B5BA-A247-AF77-BCFF49CE157A}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{40C02EE5-B5BA-A247-AF77-BCFF49CE157A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="49">
   <si>
     <t>Date</t>
   </si>
@@ -168,6 +168,21 @@
   </si>
   <si>
     <t>all_submitted_tracker_ninaSep-22-2023</t>
+  </si>
+  <si>
+    <t>master_worker_response_tracke_Sep-22-2023.csv</t>
+  </si>
+  <si>
+    <t>master_worker_response_tracke_resub_Sep-22-2023.csv</t>
+  </si>
+  <si>
+    <t>paiewise_resub</t>
+  </si>
+  <si>
+    <t>all_submitted_tracker_nina_resubSep-22-2023.csv</t>
+  </si>
+  <si>
+    <t>master_all_responses_Sep-22-2023_to_resub_Sep-22-2023_Nina.csv</t>
   </si>
 </sst>
 </file>
@@ -528,10 +543,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AFACC2C-8593-5541-A725-7B0C1E651424}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -745,6 +760,29 @@
       <c r="D12" t="s">
         <v>43</v>
       </c>
+      <c r="E12" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" t="s">
+        <v>47</v>
+      </c>
+      <c r="E13" t="s">
+        <v>45</v>
+      </c>
+      <c r="F13" t="s">
+        <v>48</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
SB, Ruan HIT launch
</commit_message>
<xml_diff>
--- a/05-Amazon_MTurk_expert_response_30cow_pairwise/results/Amazon_HIT_expert_submission_track_master.xlsx
+++ b/05-Amazon_MTurk_expert_response_30cow_pairwise/results/Amazon_HIT_expert_submission_track_master.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/skysheng/Library/CloudStorage/OneDrive-UBC/R package project and Git/lameness_rank/05-Amazon_MTurk_expert_response_30cow_pairwise/results/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ubcca-my.sharepoint.com/personal/skysheng_student_ubc_ca/Documents/R package project and Git/lameness_rank/05-Amazon_MTurk_expert_response_30cow_pairwise/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A04707D-2468-8E4C-B91A-D81291A791A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{3A04707D-2468-8E4C-B91A-D81291A791A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DC276962-318F-EB49-B8FF-5134FA5D2640}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{40C02EE5-B5BA-A247-AF77-BCFF49CE157A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="55">
   <si>
     <t>Date</t>
   </si>
@@ -183,6 +183,24 @@
   </si>
   <si>
     <t>master_all_responses_Sep-22-2023_to_resub_Sep-22-2023_Nina.csv</t>
+  </si>
+  <si>
+    <t>all_submitted_tracker_ruan_r2_Sep-30-2023.csv</t>
+  </si>
+  <si>
+    <t>Sept-30-2023</t>
+  </si>
+  <si>
+    <t>master_worker_response_tracke_ruan_r1_Sep-30-2023.csv</t>
+  </si>
+  <si>
+    <t>Oct-1-2023</t>
+  </si>
+  <si>
+    <t>SB</t>
+  </si>
+  <si>
+    <t>all_submitted_tracker_SB_Oct-01-2023.csv</t>
   </si>
 </sst>
 </file>
@@ -543,10 +561,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AFACC2C-8593-5541-A725-7B0C1E651424}">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -746,27 +764,27 @@
       <c r="D11" t="s">
         <v>36</v>
       </c>
+      <c r="E11" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>40</v>
+        <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="C12" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D12" t="s">
-        <v>43</v>
-      </c>
-      <c r="E12" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B13" t="s">
         <v>41</v>
@@ -775,13 +793,44 @@
         <v>42</v>
       </c>
       <c r="D13" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" t="s">
         <v>47</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E14" t="s">
         <v>45</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F14" t="s">
         <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SB all response collected for pairwise
</commit_message>
<xml_diff>
--- a/05-Amazon_MTurk_expert_response_30cow_pairwise/results/Amazon_HIT_expert_submission_track_master.xlsx
+++ b/05-Amazon_MTurk_expert_response_30cow_pairwise/results/Amazon_HIT_expert_submission_track_master.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ubcca-my.sharepoint.com/personal/skysheng_student_ubc_ca/Documents/R package project and Git/lameness_rank/05-Amazon_MTurk_expert_response_30cow_pairwise/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{3A04707D-2468-8E4C-B91A-D81291A791A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DC276962-318F-EB49-B8FF-5134FA5D2640}"/>
+  <xr:revisionPtr revIDLastSave="29" documentId="13_ncr:1_{3A04707D-2468-8E4C-B91A-D81291A791A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D3E54A6D-7528-974C-9A23-6C3EEE66C4DE}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{40C02EE5-B5BA-A247-AF77-BCFF49CE157A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="59">
   <si>
     <t>Date</t>
   </si>
@@ -201,6 +201,18 @@
   </si>
   <si>
     <t>all_submitted_tracker_SB_Oct-01-2023.csv</t>
+  </si>
+  <si>
+    <t>master_all_responses_SB_resub_Oct-01-2023.csv</t>
+  </si>
+  <si>
+    <t>re_submitted_tracker_SB_Oct-01-2023.csv</t>
+  </si>
+  <si>
+    <t>master_worker_response_tracke_SB_Oct-01-2023.csv</t>
+  </si>
+  <si>
+    <t>all_submitted_tracker_SB_video_no_play_Oct-01-2023.csv</t>
   </si>
 </sst>
 </file>
@@ -262,6 +274,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -561,10 +577,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AFACC2C-8593-5541-A725-7B0C1E651424}">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -832,8 +848,43 @@
       <c r="D15" t="s">
         <v>54</v>
       </c>
+      <c r="E15" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" t="s">
+        <v>53</v>
+      </c>
+      <c r="D16" t="s">
+        <v>56</v>
+      </c>
+      <c r="E16" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" t="s">
+        <v>53</v>
+      </c>
+      <c r="D17" t="s">
+        <v>58</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
SB response further process
</commit_message>
<xml_diff>
--- a/05-Amazon_MTurk_expert_response_30cow_pairwise/results/Amazon_HIT_expert_submission_track_master.xlsx
+++ b/05-Amazon_MTurk_expert_response_30cow_pairwise/results/Amazon_HIT_expert_submission_track_master.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ubcca-my.sharepoint.com/personal/skysheng_student_ubc_ca/Documents/R package project and Git/lameness_rank/05-Amazon_MTurk_expert_response_30cow_pairwise/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="29" documentId="13_ncr:1_{3A04707D-2468-8E4C-B91A-D81291A791A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D3E54A6D-7528-974C-9A23-6C3EEE66C4DE}"/>
+  <xr:revisionPtr revIDLastSave="34" documentId="13_ncr:1_{3A04707D-2468-8E4C-B91A-D81291A791A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{278973CD-0925-5F44-87DC-A7E9FAE82393}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{40C02EE5-B5BA-A247-AF77-BCFF49CE157A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="58">
   <si>
     <t>Date</t>
   </si>
@@ -98,12 +98,6 @@
     <t>master_all_responses_May-14-2023_to_May-18-2023_Dan.csv</t>
   </si>
   <si>
-    <t>pairwise_merge</t>
-  </si>
-  <si>
-    <t>May-18-2023</t>
-  </si>
-  <si>
     <t>May-29-2023</t>
   </si>
   <si>
@@ -212,7 +206,10 @@
     <t>master_worker_response_tracke_SB_Oct-01-2023.csv</t>
   </si>
   <si>
-    <t>all_submitted_tracker_SB_video_no_play_Oct-01-2023.csv</t>
+    <t>master_all_responses_Jun-19-2023_to_Jul-14-2023_Wali.csv</t>
+  </si>
+  <si>
+    <t>master_all_responses_SB_Oct-01-2023_to_SB_resub_Oct-01-2023_Sarah.csv</t>
   </si>
 </sst>
 </file>
@@ -274,10 +271,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -577,10 +570,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AFACC2C-8593-5541-A725-7B0C1E651424}">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -611,10 +604,10 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -625,7 +618,7 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>
@@ -642,7 +635,7 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D3" t="s">
         <v>8</v>
@@ -653,13 +646,13 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D4" t="s">
         <v>10</v>
@@ -670,13 +663,13 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B5" t="s">
         <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D5" t="s">
         <v>13</v>
@@ -687,13 +680,13 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B6" t="s">
         <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D6" t="s">
         <v>16</v>
@@ -701,70 +694,79 @@
       <c r="E6" t="s">
         <v>18</v>
       </c>
+      <c r="F6" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
         <v>20</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" t="s">
         <v>21</v>
       </c>
-      <c r="C7" t="s">
-        <v>37</v>
-      </c>
       <c r="E7" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D8" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="E8" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B9" t="s">
         <v>26</v>
       </c>
       <c r="C9" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E9" t="s">
-        <v>32</v>
+        <v>31</v>
+      </c>
+      <c r="F9" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>31</v>
+        <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="C10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D10" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="E10" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -772,115 +774,87 @@
         <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="C11" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D11" t="s">
-        <v>36</v>
-      </c>
-      <c r="E11" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>5</v>
+        <v>38</v>
       </c>
       <c r="B12" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="C12" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D12" t="s">
-        <v>49</v>
+        <v>41</v>
+      </c>
+      <c r="E12" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" t="s">
         <v>40</v>
       </c>
-      <c r="B13" t="s">
-        <v>41</v>
-      </c>
-      <c r="C13" t="s">
-        <v>42</v>
-      </c>
       <c r="D13" t="s">
+        <v>45</v>
+      </c>
+      <c r="E13" t="s">
         <v>43</v>
       </c>
-      <c r="E13" t="s">
-        <v>44</v>
+      <c r="F13" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B14" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="C14" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="D14" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="E14" t="s">
-        <v>45</v>
-      </c>
-      <c r="F14" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B15" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C15" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D15" t="s">
         <v>54</v>
       </c>
       <c r="E15" t="s">
+        <v>53</v>
+      </c>
+      <c r="F15" t="s">
         <v>57</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>46</v>
-      </c>
-      <c r="B16" t="s">
-        <v>52</v>
-      </c>
-      <c r="C16" t="s">
-        <v>53</v>
-      </c>
-      <c r="D16" t="s">
-        <v>56</v>
-      </c>
-      <c r="E16" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>31</v>
-      </c>
-      <c r="B17" t="s">
-        <v>52</v>
-      </c>
-      <c r="C17" t="s">
-        <v>53</v>
-      </c>
-      <c r="D17" t="s">
-        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TM expert response collect
</commit_message>
<xml_diff>
--- a/05-Amazon_MTurk_expert_response_30cow_pairwise/results/Amazon_HIT_expert_submission_track_master.xlsx
+++ b/05-Amazon_MTurk_expert_response_30cow_pairwise/results/Amazon_HIT_expert_submission_track_master.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ubcca-my.sharepoint.com/personal/skysheng_student_ubc_ca/Documents/R package project and Git/lameness_rank/05-Amazon_MTurk_expert_response_30cow_pairwise/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="34" documentId="13_ncr:1_{3A04707D-2468-8E4C-B91A-D81291A791A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{278973CD-0925-5F44-87DC-A7E9FAE82393}"/>
+  <xr:revisionPtr revIDLastSave="38" documentId="13_ncr:1_{3A04707D-2468-8E4C-B91A-D81291A791A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9EEA6CCF-E570-0649-A567-294BC930C11C}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{40C02EE5-B5BA-A247-AF77-BCFF49CE157A}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17180" xr2:uid="{40C02EE5-B5BA-A247-AF77-BCFF49CE157A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="61">
   <si>
     <t>Date</t>
   </si>
@@ -210,6 +210,15 @@
   </si>
   <si>
     <t>master_all_responses_SB_Oct-01-2023_to_SB_resub_Oct-01-2023_Sarah.csv</t>
+  </si>
+  <si>
+    <t>TM</t>
+  </si>
+  <si>
+    <t>Oct-24-2023</t>
+  </si>
+  <si>
+    <t>all_submitted_tracker_TM_Oct-24-2023.csv</t>
   </si>
 </sst>
 </file>
@@ -570,10 +579,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AFACC2C-8593-5541-A725-7B0C1E651424}">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -857,6 +866,20 @@
         <v>57</v>
       </c>
     </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" t="s">
+        <v>58</v>
+      </c>
+      <c r="D16" t="s">
+        <v>60</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
RD expert new link relaunch
</commit_message>
<xml_diff>
--- a/05-Amazon_MTurk_expert_response_30cow_pairwise/results/Amazon_HIT_expert_submission_track_master.xlsx
+++ b/05-Amazon_MTurk_expert_response_30cow_pairwise/results/Amazon_HIT_expert_submission_track_master.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ubcca-my.sharepoint.com/personal/skysheng_student_ubc_ca/Documents/R package project and Git/lameness_rank/05-Amazon_MTurk_expert_response_30cow_pairwise/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="58" documentId="13_ncr:1_{3A04707D-2468-8E4C-B91A-D81291A791A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F18E5E72-F664-D143-9D0D-86D73BB97216}"/>
+  <xr:revisionPtr revIDLastSave="62" documentId="13_ncr:1_{3A04707D-2468-8E4C-B91A-D81291A791A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CD4F308D-D9D4-934E-800D-EB73A4FD886D}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{40C02EE5-B5BA-A247-AF77-BCFF49CE157A}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17180" xr2:uid="{40C02EE5-B5BA-A247-AF77-BCFF49CE157A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="61">
   <si>
     <t>Date</t>
   </si>
@@ -213,6 +213,12 @@
   </si>
   <si>
     <t>master_all_responses_KINov-11-2023_to_KI_resub2Nov-11-2023_Kiyomi.csv</t>
+  </si>
+  <si>
+    <t>all_submitted_tracker_RD_Nov-20-2023.csv</t>
+  </si>
+  <si>
+    <t>Nov-20-2023</t>
   </si>
 </sst>
 </file>
@@ -274,10 +280,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -577,10 +579,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AFACC2C-8593-5541-A725-7B0C1E651424}">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -881,6 +883,20 @@
         <v>58</v>
       </c>
     </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" t="s">
+        <v>60</v>
+      </c>
+      <c r="C17" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" t="s">
+        <v>59</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>